<commit_message>
adding test ng test cases
</commit_message>
<xml_diff>
--- a/webTableToExcel.xlsx
+++ b/webTableToExcel.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
   <si>
     <t>Name</t>
   </si>
@@ -41,12 +41,19 @@
   </si>
   <si>
     <t>a</t>
+  </si>
+  <si>
+    <t>bh</t>
+  </si>
+  <si>
+    <t>Piyali</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -364,7 +371,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
@@ -372,7 +379,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.0" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -419,6 +426,16 @@
         <v>8</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>